<commit_message>
Changed APGAR in Children.xlsx
</commit_message>
<xml_diff>
--- a/Children.xlsx
+++ b/Children.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>СРАР</t>
   </si>
@@ -513,19 +513,23 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19.109375" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="10" max="10" width="10" customWidth="1"/>
-    <col min="11" max="11" width="18.21875" customWidth="1"/>
-    <col min="12" max="12" width="22" customWidth="1"/>
-    <col min="13" max="13" width="12.5546875" customWidth="1"/>
-    <col min="14" max="14" width="15.33203125" customWidth="1"/>
-    <col min="16" max="16" width="17.109375" customWidth="1"/>
+    <col min="8" max="8" width="6.77734375" customWidth="1"/>
+    <col min="9" max="9" width="5.21875" customWidth="1"/>
+    <col min="10" max="10" width="6.44140625" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" customWidth="1"/>
+    <col min="12" max="12" width="17" customWidth="1"/>
+    <col min="13" max="13" width="21" customWidth="1"/>
+    <col min="14" max="14" width="11.88671875" customWidth="1"/>
+    <col min="15" max="15" width="9.21875" customWidth="1"/>
+    <col min="16" max="16" width="7.5546875" customWidth="1"/>
+    <col min="17" max="17" width="15.88671875" customWidth="1"/>
     <col min="23" max="23" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -548,34 +552,37 @@
       <c r="F1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="11" t="s">
-        <v>0</v>
+      <c r="G1" s="12" t="s">
+        <v>8</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="P1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
         <v>30</v>
       </c>
     </row>
@@ -596,14 +603,13 @@
         <v>35</v>
       </c>
       <c r="F2" s="5">
-        <f>5/6</f>
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="G2" s="2">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="G2" s="5">
+        <v>6</v>
       </c>
       <c r="H2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" s="2">
         <v>0</v>
@@ -611,22 +617,25 @@
       <c r="J2" s="2">
         <v>0</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K2" s="2">
         <v>0</v>
       </c>
       <c r="L2" s="6">
         <v>0</v>
       </c>
-      <c r="M2" s="1">
-        <v>0</v>
-      </c>
-      <c r="N2" s="8">
+      <c r="M2" s="6">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
         <v>0</v>
       </c>
       <c r="O2" s="8">
         <v>0</v>
       </c>
       <c r="P2" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="8">
         <v>0</v>
       </c>
       <c r="R2" s="10"/>
@@ -648,14 +657,13 @@
         <v>40</v>
       </c>
       <c r="F3" s="5">
-        <f>4/5</f>
-        <v>0.8</v>
-      </c>
-      <c r="G3" s="2">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="G3" s="5">
+        <v>5</v>
       </c>
       <c r="H3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="2">
         <v>0</v>
@@ -663,22 +671,25 @@
       <c r="J3" s="2">
         <v>0</v>
       </c>
-      <c r="K3" s="6">
-        <v>1</v>
+      <c r="K3" s="2">
+        <v>0</v>
       </c>
       <c r="L3" s="6">
         <v>1</v>
       </c>
-      <c r="M3" s="1">
-        <v>0</v>
-      </c>
-      <c r="N3" s="8">
+      <c r="M3" s="6">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1">
         <v>0</v>
       </c>
       <c r="O3" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P3" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="8">
         <v>0</v>
       </c>
       <c r="R3" s="9"/>
@@ -700,37 +711,39 @@
         <v>33</v>
       </c>
       <c r="F4" s="5">
-        <f>2/3</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="G4" s="5">
+        <v>3</v>
       </c>
       <c r="H4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="2">
         <v>0</v>
       </c>
-      <c r="K4" s="6">
-        <v>1</v>
+      <c r="K4" s="2">
+        <v>0</v>
       </c>
       <c r="L4" s="6">
         <v>1</v>
       </c>
-      <c r="M4" s="1">
-        <v>1</v>
-      </c>
-      <c r="N4" s="8">
-        <v>0</v>
+      <c r="M4" s="6">
+        <v>1</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1</v>
       </c>
       <c r="O4" s="8">
         <v>0</v>
       </c>
       <c r="P4" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="8">
         <v>0</v>
       </c>
       <c r="R4" s="9"/>
@@ -752,37 +765,39 @@
         <v>44</v>
       </c>
       <c r="F5" s="5">
-        <f>6/6</f>
-        <v>1</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="G5" s="5">
+        <v>6</v>
       </c>
       <c r="H5" s="2">
         <v>0</v>
       </c>
-      <c r="I5" s="4">
-        <v>1</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0</v>
-      </c>
-      <c r="K5" s="6">
-        <v>1</v>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
       </c>
       <c r="L5" s="6">
         <v>1</v>
       </c>
-      <c r="M5" s="1">
-        <v>1</v>
-      </c>
-      <c r="N5" s="8">
-        <v>0</v>
+      <c r="M5" s="6">
+        <v>1</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1</v>
       </c>
       <c r="O5" s="8">
         <v>0</v>
       </c>
       <c r="P5" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="8">
         <v>0</v>
       </c>
       <c r="R5" s="9"/>
@@ -804,37 +819,39 @@
         <v>43</v>
       </c>
       <c r="F6" s="5">
-        <f>3/5</f>
-        <v>0.6</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="G6" s="5">
+        <v>5</v>
       </c>
       <c r="H6" s="2">
         <v>0</v>
       </c>
-      <c r="I6" s="4">
-        <v>1</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0</v>
-      </c>
-      <c r="K6" s="6">
-        <v>1</v>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
       </c>
       <c r="L6" s="6">
         <v>1</v>
       </c>
-      <c r="M6" s="1">
-        <v>1</v>
-      </c>
-      <c r="N6" s="8">
-        <v>0</v>
+      <c r="M6" s="6">
+        <v>1</v>
+      </c>
+      <c r="N6" s="1">
+        <v>1</v>
       </c>
       <c r="O6" s="8">
         <v>0</v>
       </c>
       <c r="P6" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="8">
         <v>0</v>
       </c>
       <c r="R6" s="9"/>
@@ -856,14 +873,13 @@
         <v>37</v>
       </c>
       <c r="F7" s="5">
-        <f>4/6</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="G7" s="2">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="G7" s="5">
+        <v>6</v>
       </c>
       <c r="H7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="2">
         <v>0</v>
@@ -871,22 +887,25 @@
       <c r="J7" s="2">
         <v>0</v>
       </c>
-      <c r="K7" s="6">
-        <v>1</v>
+      <c r="K7" s="2">
+        <v>0</v>
       </c>
       <c r="L7" s="6">
-        <v>0</v>
-      </c>
-      <c r="M7" s="1">
-        <v>0</v>
-      </c>
-      <c r="N7" s="8">
+        <v>1</v>
+      </c>
+      <c r="M7" s="6">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
         <v>0</v>
       </c>
       <c r="O7" s="8">
         <v>0</v>
       </c>
       <c r="P7" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="8">
         <v>1</v>
       </c>
       <c r="R7" s="9"/>
@@ -908,14 +927,13 @@
         <v>36</v>
       </c>
       <c r="F8" s="5">
-        <f>5/6</f>
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="G8" s="2">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="G8" s="5">
+        <v>6</v>
       </c>
       <c r="H8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="2">
         <v>0</v>
@@ -923,22 +941,25 @@
       <c r="J8" s="2">
         <v>0</v>
       </c>
-      <c r="K8" s="6">
-        <v>1</v>
+      <c r="K8" s="2">
+        <v>0</v>
       </c>
       <c r="L8" s="6">
-        <v>0</v>
-      </c>
-      <c r="M8" s="1">
-        <v>0</v>
-      </c>
-      <c r="N8" s="8">
+        <v>1</v>
+      </c>
+      <c r="M8" s="6">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1">
         <v>0</v>
       </c>
       <c r="O8" s="8">
         <v>0</v>
       </c>
       <c r="P8" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="8">
         <v>1</v>
       </c>
       <c r="R8" s="9"/>
@@ -960,14 +981,13 @@
         <v>33</v>
       </c>
       <c r="F9" s="5">
-        <f>4/6</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="G9" s="2">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="G9" s="5">
+        <v>6</v>
       </c>
       <c r="H9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="2">
         <v>0</v>
@@ -975,22 +995,25 @@
       <c r="J9" s="2">
         <v>0</v>
       </c>
-      <c r="K9" s="6">
-        <v>1</v>
+      <c r="K9" s="2">
+        <v>0</v>
       </c>
       <c r="L9" s="6">
         <v>1</v>
       </c>
-      <c r="M9" s="1">
-        <v>0</v>
-      </c>
-      <c r="N9" s="8">
+      <c r="M9" s="6">
+        <v>1</v>
+      </c>
+      <c r="N9" s="1">
         <v>0</v>
       </c>
       <c r="O9" s="8">
         <v>0</v>
       </c>
       <c r="P9" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="8">
         <v>1</v>
       </c>
       <c r="R9" s="9"/>
@@ -1012,14 +1035,13 @@
         <v>40</v>
       </c>
       <c r="F10" s="5">
-        <f>5/6</f>
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="G10" s="2">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="G10" s="5">
+        <v>6</v>
       </c>
       <c r="H10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="2">
         <v>0</v>
@@ -1027,22 +1049,25 @@
       <c r="J10" s="2">
         <v>0</v>
       </c>
-      <c r="K10" s="6">
-        <v>1</v>
+      <c r="K10" s="2">
+        <v>0</v>
       </c>
       <c r="L10" s="6">
         <v>1</v>
       </c>
-      <c r="M10" s="1">
-        <v>1</v>
-      </c>
-      <c r="N10" s="8">
-        <v>0</v>
+      <c r="M10" s="6">
+        <v>1</v>
+      </c>
+      <c r="N10" s="1">
+        <v>1</v>
       </c>
       <c r="O10" s="8">
         <v>0</v>
       </c>
       <c r="P10" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="8">
         <v>0</v>
       </c>
       <c r="R10" s="9"/>
@@ -1064,13 +1089,13 @@
         <v>40</v>
       </c>
       <c r="F11" s="5">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="G11" s="2">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="G11" s="5">
+        <v>6</v>
       </c>
       <c r="H11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="2">
         <v>0</v>
@@ -1078,22 +1103,25 @@
       <c r="J11" s="2">
         <v>0</v>
       </c>
-      <c r="K11" s="6">
-        <v>1</v>
+      <c r="K11" s="2">
+        <v>0</v>
       </c>
       <c r="L11" s="6">
         <v>1</v>
       </c>
-      <c r="M11" s="1">
-        <v>1</v>
-      </c>
-      <c r="N11" s="8">
-        <v>0</v>
+      <c r="M11" s="6">
+        <v>1</v>
+      </c>
+      <c r="N11" s="1">
+        <v>1</v>
       </c>
       <c r="O11" s="8">
         <v>0</v>
       </c>
       <c r="P11" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="8">
         <v>0</v>
       </c>
       <c r="R11" s="9"/>
@@ -1115,37 +1143,39 @@
         <v>35</v>
       </c>
       <c r="F12" s="5">
-        <f>4/6</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="G12" s="5">
+        <v>4</v>
       </c>
       <c r="H12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="2">
         <v>0</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K12" s="2">
         <v>0</v>
       </c>
       <c r="L12" s="6">
         <v>0</v>
       </c>
-      <c r="M12" s="1">
-        <v>0</v>
-      </c>
-      <c r="N12" s="8">
+      <c r="M12" s="6">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1">
         <v>0</v>
       </c>
       <c r="O12" s="8">
         <v>0</v>
       </c>
       <c r="P12" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="8">
         <v>0</v>
       </c>
       <c r="R12" s="10"/>
@@ -1167,37 +1197,39 @@
         <v>21</v>
       </c>
       <c r="F13" s="5">
-        <f>2/4</f>
-        <v>0.5</v>
-      </c>
-      <c r="G13" s="2">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="G13" s="5">
+        <v>2</v>
       </c>
       <c r="H13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" s="2">
         <v>0</v>
       </c>
-      <c r="K13" s="6">
+      <c r="K13" s="2">
         <v>0</v>
       </c>
       <c r="L13" s="6">
         <v>0</v>
       </c>
-      <c r="M13" s="1">
-        <v>0</v>
-      </c>
-      <c r="N13" s="8">
+      <c r="M13" s="6">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
         <v>0</v>
       </c>
       <c r="O13" s="8">
         <v>0</v>
       </c>
       <c r="P13" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="8">
         <v>0</v>
       </c>
       <c r="R13" s="10"/>
@@ -1219,37 +1251,39 @@
         <v>38</v>
       </c>
       <c r="F14" s="5">
-        <f>3/5</f>
-        <v>0.6</v>
-      </c>
-      <c r="G14" s="2">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="G14" s="5">
+        <v>3</v>
       </c>
       <c r="H14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" s="2">
         <v>0</v>
       </c>
-      <c r="K14" s="6">
+      <c r="K14" s="2">
         <v>0</v>
       </c>
       <c r="L14" s="6">
         <v>0</v>
       </c>
-      <c r="M14" s="1">
-        <v>0</v>
-      </c>
-      <c r="N14" s="8">
+      <c r="M14" s="6">
+        <v>0</v>
+      </c>
+      <c r="N14" s="1">
         <v>0</v>
       </c>
       <c r="O14" s="8">
         <v>0</v>
       </c>
       <c r="P14" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="8">
         <v>0</v>
       </c>
       <c r="R14" s="10"/>
@@ -1271,14 +1305,13 @@
         <v>40</v>
       </c>
       <c r="F15" s="5">
-        <f>4/6</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="G15" s="2">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="G15" s="5">
+        <v>4</v>
       </c>
       <c r="H15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="2">
         <v>0</v>
@@ -1286,22 +1319,25 @@
       <c r="J15" s="2">
         <v>0</v>
       </c>
-      <c r="K15" s="6">
-        <v>1</v>
+      <c r="K15" s="2">
+        <v>0</v>
       </c>
       <c r="L15" s="6">
         <v>1</v>
       </c>
-      <c r="M15" s="1">
-        <v>0</v>
-      </c>
-      <c r="N15" s="8">
+      <c r="M15" s="6">
+        <v>1</v>
+      </c>
+      <c r="N15" s="1">
         <v>0</v>
       </c>
       <c r="O15" s="8">
         <v>0</v>
       </c>
       <c r="P15" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="8">
         <v>1</v>
       </c>
       <c r="R15" s="9"/>
@@ -1323,14 +1359,13 @@
         <v>40</v>
       </c>
       <c r="F16" s="5">
-        <f>4/6</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="G16" s="2">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="G16" s="5">
+        <v>4</v>
       </c>
       <c r="H16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="2">
         <v>0</v>
@@ -1338,22 +1373,25 @@
       <c r="J16" s="2">
         <v>0</v>
       </c>
-      <c r="K16" s="6">
-        <v>1</v>
+      <c r="K16" s="2">
+        <v>0</v>
       </c>
       <c r="L16" s="6">
         <v>1</v>
       </c>
-      <c r="M16" s="1">
-        <v>0</v>
-      </c>
-      <c r="N16" s="8">
+      <c r="M16" s="6">
+        <v>1</v>
+      </c>
+      <c r="N16" s="1">
         <v>0</v>
       </c>
       <c r="O16" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P16" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="8">
         <v>0</v>
       </c>
       <c r="R16" s="9"/>
@@ -1375,11 +1413,10 @@
         <v>39</v>
       </c>
       <c r="F17" s="5">
-        <f>3/4</f>
-        <v>0.75</v>
-      </c>
-      <c r="G17" s="2">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="G17" s="5">
+        <v>3</v>
       </c>
       <c r="H17" s="2">
         <v>0</v>
@@ -1387,25 +1424,28 @@
       <c r="I17" s="2">
         <v>0</v>
       </c>
-      <c r="J17" s="4">
-        <v>1</v>
-      </c>
-      <c r="K17" s="6">
-        <v>0</v>
+      <c r="J17" s="2">
+        <v>0</v>
+      </c>
+      <c r="K17" s="4">
+        <v>1</v>
       </c>
       <c r="L17" s="6">
         <v>0</v>
       </c>
-      <c r="M17" s="1">
-        <v>0</v>
-      </c>
-      <c r="N17" s="8">
+      <c r="M17" s="6">
+        <v>0</v>
+      </c>
+      <c r="N17" s="1">
         <v>0</v>
       </c>
       <c r="O17" s="8">
         <v>0</v>
       </c>
       <c r="P17" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="8">
         <v>0</v>
       </c>
       <c r="R17" s="10"/>
@@ -1427,14 +1467,13 @@
         <v>39</v>
       </c>
       <c r="F18" s="5">
-        <f>5/6</f>
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="G18" s="2">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="G18" s="5">
+        <v>5</v>
       </c>
       <c r="H18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="2">
         <v>0</v>
@@ -1442,22 +1481,25 @@
       <c r="J18" s="2">
         <v>0</v>
       </c>
-      <c r="K18" s="6">
-        <v>1</v>
+      <c r="K18" s="2">
+        <v>0</v>
       </c>
       <c r="L18" s="6">
-        <v>0</v>
-      </c>
-      <c r="M18" s="1">
-        <v>0</v>
-      </c>
-      <c r="N18" s="8">
+        <v>1</v>
+      </c>
+      <c r="M18" s="6">
+        <v>0</v>
+      </c>
+      <c r="N18" s="1">
         <v>0</v>
       </c>
       <c r="O18" s="8">
         <v>0</v>
       </c>
       <c r="P18" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="8">
         <v>1</v>
       </c>
       <c r="R18" s="9"/>

</xml_diff>

<commit_message>
Changed output and *.xlsx file
</commit_message>
<xml_diff>
--- a/Children.xlsx
+++ b/Children.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>СРАР</t>
   </si>
@@ -47,9 +47,6 @@
     <t>длина</t>
   </si>
   <si>
-    <t>Апгар</t>
-  </si>
-  <si>
     <t>ВЧО-ИВЛ</t>
   </si>
   <si>
@@ -101,19 +98,25 @@
     <t>18.2.2018</t>
   </si>
   <si>
-    <t>Физическое развитие</t>
-  </si>
-  <si>
     <t>Норма НПР</t>
   </si>
   <si>
-    <t>Моторика</t>
-  </si>
-  <si>
-    <t>Речь</t>
-  </si>
-  <si>
-    <t>Моторика + речь</t>
+    <t>Апгар(1 мин)</t>
+  </si>
+  <si>
+    <t>Апгар(5 мин)</t>
+  </si>
+  <si>
+    <t>Задержка моторика</t>
+  </si>
+  <si>
+    <t>Задержка речь</t>
+  </si>
+  <si>
+    <t>Задержка моторика + речь</t>
+  </si>
+  <si>
+    <t>Норма физ. Развития</t>
   </si>
 </sst>
 </file>
@@ -513,13 +516,16 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.109375" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="6.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="6.77734375" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" customWidth="1"/>
     <col min="8" max="8" width="6.77734375" customWidth="1"/>
     <col min="9" max="9" width="5.21875" customWidth="1"/>
     <col min="10" max="10" width="6.44140625" customWidth="1"/>
@@ -527,9 +533,9 @@
     <col min="12" max="12" width="17" customWidth="1"/>
     <col min="13" max="13" width="21" customWidth="1"/>
     <col min="14" max="14" width="11.88671875" customWidth="1"/>
-    <col min="15" max="15" width="9.21875" customWidth="1"/>
-    <col min="16" max="16" width="7.5546875" customWidth="1"/>
-    <col min="17" max="17" width="15.88671875" customWidth="1"/>
+    <col min="15" max="15" width="18.44140625" customWidth="1"/>
+    <col min="16" max="16" width="14.21875" customWidth="1"/>
+    <col min="17" max="17" width="24.44140625" customWidth="1"/>
     <col min="23" max="23" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -550,10 +556,10 @@
         <v>7</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>0</v>
@@ -565,16 +571,16 @@
         <v>2</v>
       </c>
       <c r="K1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="11" t="s">
-        <v>10</v>
-      </c>
       <c r="M1" s="11" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O1" s="11" t="s">
         <v>28</v>
@@ -591,7 +597,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3">
         <v>29</v>
@@ -645,7 +651,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3">
         <v>32</v>
@@ -699,7 +705,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3">
         <v>28</v>
@@ -753,7 +759,7 @@
         <v>29</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3">
         <v>31</v>
@@ -807,7 +813,7 @@
         <v>30</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="3">
         <v>31</v>
@@ -861,7 +867,7 @@
         <v>35</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="3">
         <v>31</v>
@@ -915,7 +921,7 @@
         <v>38</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="3">
         <v>29</v>
@@ -969,7 +975,7 @@
         <v>40</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="3">
         <v>27</v>
@@ -1023,7 +1029,7 @@
         <v>41</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="3">
         <v>30</v>
@@ -1077,7 +1083,7 @@
         <v>42</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="3">
         <v>30</v>
@@ -1131,7 +1137,7 @@
         <v>76</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="3">
         <v>27</v>
@@ -1185,7 +1191,7 @@
         <v>120</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="3">
         <v>25</v>
@@ -1239,7 +1245,7 @@
         <v>139</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="3">
         <v>29</v>
@@ -1293,7 +1299,7 @@
         <v>148</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" s="3">
         <v>28</v>
@@ -1347,7 +1353,7 @@
         <v>156</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="3">
         <v>31</v>
@@ -1401,7 +1407,7 @@
         <v>160</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="3">
         <v>29</v>
@@ -1455,7 +1461,7 @@
         <v>170</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" s="3">
         <v>30</v>

</xml_diff>

<commit_message>
Column width changed in *.xlsx
</commit_message>
<xml_diff>
--- a/Children.xlsx
+++ b/Children.xlsx
@@ -35,9 +35,6 @@
     <t>№</t>
   </si>
   <si>
-    <t>Дата рождения</t>
-  </si>
-  <si>
     <t>ГВ</t>
   </si>
   <si>
@@ -107,16 +104,19 @@
     <t>Апгар(5 мин)</t>
   </si>
   <si>
-    <t>Задержка моторика</t>
-  </si>
-  <si>
-    <t>Задержка речь</t>
-  </si>
-  <si>
-    <t>Задержка моторика + речь</t>
-  </si>
-  <si>
-    <t>Норма физ. Развития</t>
+    <t>Норма ФР</t>
+  </si>
+  <si>
+    <t>Задерж.мот.</t>
+  </si>
+  <si>
+    <t>Задерж.речь</t>
+  </si>
+  <si>
+    <t>Задер.моторика+речь</t>
+  </si>
+  <si>
+    <t>Дата рожд.</t>
   </si>
 </sst>
 </file>
@@ -176,7 +176,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -185,7 +185,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -516,79 +515,81 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.109375" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="6.77734375" customWidth="1"/>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="4.6640625" customWidth="1"/>
+    <col min="4" max="4" width="7.21875" customWidth="1"/>
+    <col min="5" max="5" width="7.109375" customWidth="1"/>
     <col min="6" max="6" width="11.44140625" customWidth="1"/>
     <col min="7" max="7" width="11.77734375" customWidth="1"/>
-    <col min="8" max="8" width="6.77734375" customWidth="1"/>
-    <col min="9" max="9" width="5.21875" customWidth="1"/>
-    <col min="10" max="10" width="6.44140625" customWidth="1"/>
-    <col min="11" max="11" width="10.44140625" customWidth="1"/>
+    <col min="8" max="8" width="5.77734375" customWidth="1"/>
+    <col min="9" max="9" width="4.5546875" customWidth="1"/>
+    <col min="10" max="10" width="4.77734375" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" customWidth="1"/>
     <col min="12" max="12" width="17" customWidth="1"/>
-    <col min="13" max="13" width="21" customWidth="1"/>
-    <col min="14" max="14" width="11.88671875" customWidth="1"/>
-    <col min="15" max="15" width="18.44140625" customWidth="1"/>
-    <col min="16" max="16" width="14.21875" customWidth="1"/>
-    <col min="17" max="17" width="24.44140625" customWidth="1"/>
+    <col min="13" max="13" width="9.44140625" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" customWidth="1"/>
+    <col min="15" max="15" width="11.109375" customWidth="1"/>
+    <col min="16" max="16" width="11.5546875" customWidth="1"/>
+    <col min="17" max="17" width="20" customWidth="1"/>
     <col min="23" max="23" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="13" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:18" s="12" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="12" t="s">
+      <c r="L1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" s="11" t="s">
+      <c r="N1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="Q1" s="10" t="s">
         <v>30</v>
       </c>
     </row>
@@ -596,8 +597,8 @@
       <c r="A2" s="2">
         <v>25</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>10</v>
+      <c r="B2" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C2" s="3">
         <v>29</v>
@@ -626,32 +627,32 @@
       <c r="K2" s="2">
         <v>0</v>
       </c>
-      <c r="L2" s="6">
-        <v>0</v>
-      </c>
-      <c r="M2" s="6">
+      <c r="L2" s="7">
+        <v>0</v>
+      </c>
+      <c r="M2" s="7">
         <v>0</v>
       </c>
       <c r="N2" s="1">
         <v>0</v>
       </c>
-      <c r="O2" s="8">
-        <v>0</v>
-      </c>
-      <c r="P2" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="8">
-        <v>0</v>
-      </c>
-      <c r="R2" s="10"/>
+      <c r="O2" s="7">
+        <v>0</v>
+      </c>
+      <c r="P2" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="7">
+        <v>0</v>
+      </c>
+      <c r="R2" s="9"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>26</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>11</v>
+      <c r="B3" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="C3" s="3">
         <v>32</v>
@@ -680,32 +681,32 @@
       <c r="K3" s="2">
         <v>0</v>
       </c>
-      <c r="L3" s="6">
-        <v>1</v>
-      </c>
-      <c r="M3" s="6">
+      <c r="L3" s="7">
+        <v>1</v>
+      </c>
+      <c r="M3" s="7">
         <v>1</v>
       </c>
       <c r="N3" s="1">
         <v>0</v>
       </c>
-      <c r="O3" s="8">
-        <v>0</v>
-      </c>
-      <c r="P3" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="8">
-        <v>0</v>
-      </c>
-      <c r="R3" s="9"/>
+      <c r="O3" s="7">
+        <v>0</v>
+      </c>
+      <c r="P3" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>0</v>
+      </c>
+      <c r="R3" s="8"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>27</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>12</v>
+      <c r="B4" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="C4" s="3">
         <v>28</v>
@@ -734,32 +735,32 @@
       <c r="K4" s="2">
         <v>0</v>
       </c>
-      <c r="L4" s="6">
-        <v>1</v>
-      </c>
-      <c r="M4" s="6">
+      <c r="L4" s="7">
+        <v>1</v>
+      </c>
+      <c r="M4" s="7">
         <v>1</v>
       </c>
       <c r="N4" s="1">
         <v>1</v>
       </c>
-      <c r="O4" s="8">
-        <v>0</v>
-      </c>
-      <c r="P4" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="8">
-        <v>0</v>
-      </c>
-      <c r="R4" s="9"/>
+      <c r="O4" s="7">
+        <v>0</v>
+      </c>
+      <c r="P4" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>0</v>
+      </c>
+      <c r="R4" s="8"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>29</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>13</v>
+      <c r="B5" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="C5" s="3">
         <v>31</v>
@@ -788,32 +789,32 @@
       <c r="K5" s="2">
         <v>0</v>
       </c>
-      <c r="L5" s="6">
-        <v>1</v>
-      </c>
-      <c r="M5" s="6">
+      <c r="L5" s="7">
+        <v>1</v>
+      </c>
+      <c r="M5" s="7">
         <v>1</v>
       </c>
       <c r="N5" s="1">
         <v>1</v>
       </c>
-      <c r="O5" s="8">
-        <v>0</v>
-      </c>
-      <c r="P5" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="8">
-        <v>0</v>
-      </c>
-      <c r="R5" s="9"/>
+      <c r="O5" s="7">
+        <v>0</v>
+      </c>
+      <c r="P5" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>0</v>
+      </c>
+      <c r="R5" s="8"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>30</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>13</v>
+      <c r="B6" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="C6" s="3">
         <v>31</v>
@@ -842,32 +843,32 @@
       <c r="K6" s="2">
         <v>0</v>
       </c>
-      <c r="L6" s="6">
-        <v>1</v>
-      </c>
-      <c r="M6" s="6">
+      <c r="L6" s="7">
+        <v>1</v>
+      </c>
+      <c r="M6" s="7">
         <v>1</v>
       </c>
       <c r="N6" s="1">
         <v>1</v>
       </c>
-      <c r="O6" s="8">
-        <v>0</v>
-      </c>
-      <c r="P6" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="8">
-        <v>0</v>
-      </c>
-      <c r="R6" s="9"/>
+      <c r="O6" s="7">
+        <v>0</v>
+      </c>
+      <c r="P6" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="7">
+        <v>0</v>
+      </c>
+      <c r="R6" s="8"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>35</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>14</v>
+      <c r="B7" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="C7" s="3">
         <v>31</v>
@@ -896,32 +897,32 @@
       <c r="K7" s="2">
         <v>0</v>
       </c>
-      <c r="L7" s="6">
-        <v>1</v>
-      </c>
-      <c r="M7" s="6">
+      <c r="L7" s="7">
+        <v>1</v>
+      </c>
+      <c r="M7" s="7">
         <v>0</v>
       </c>
       <c r="N7" s="1">
         <v>0</v>
       </c>
-      <c r="O7" s="8">
-        <v>0</v>
-      </c>
-      <c r="P7" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="8">
-        <v>1</v>
-      </c>
-      <c r="R7" s="9"/>
+      <c r="O7" s="7">
+        <v>0</v>
+      </c>
+      <c r="P7" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>1</v>
+      </c>
+      <c r="R7" s="8"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>38</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>15</v>
+      <c r="B8" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C8" s="3">
         <v>29</v>
@@ -950,32 +951,32 @@
       <c r="K8" s="2">
         <v>0</v>
       </c>
-      <c r="L8" s="6">
-        <v>1</v>
-      </c>
-      <c r="M8" s="6">
+      <c r="L8" s="7">
+        <v>1</v>
+      </c>
+      <c r="M8" s="7">
         <v>0</v>
       </c>
       <c r="N8" s="1">
         <v>0</v>
       </c>
-      <c r="O8" s="8">
-        <v>0</v>
-      </c>
-      <c r="P8" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="8">
-        <v>1</v>
-      </c>
-      <c r="R8" s="9"/>
+      <c r="O8" s="7">
+        <v>0</v>
+      </c>
+      <c r="P8" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="7">
+        <v>1</v>
+      </c>
+      <c r="R8" s="8"/>
     </row>
     <row r="9" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>40</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>16</v>
+      <c r="B9" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="C9" s="3">
         <v>27</v>
@@ -1004,32 +1005,32 @@
       <c r="K9" s="2">
         <v>0</v>
       </c>
-      <c r="L9" s="6">
-        <v>1</v>
-      </c>
-      <c r="M9" s="6">
+      <c r="L9" s="7">
+        <v>1</v>
+      </c>
+      <c r="M9" s="7">
         <v>1</v>
       </c>
       <c r="N9" s="1">
         <v>0</v>
       </c>
-      <c r="O9" s="8">
-        <v>0</v>
-      </c>
-      <c r="P9" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="8">
-        <v>1</v>
-      </c>
-      <c r="R9" s="9"/>
+      <c r="O9" s="7">
+        <v>0</v>
+      </c>
+      <c r="P9" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="7">
+        <v>1</v>
+      </c>
+      <c r="R9" s="8"/>
     </row>
     <row r="10" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>41</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>17</v>
+      <c r="B10" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="C10" s="3">
         <v>30</v>
@@ -1058,32 +1059,32 @@
       <c r="K10" s="2">
         <v>0</v>
       </c>
-      <c r="L10" s="6">
-        <v>1</v>
-      </c>
-      <c r="M10" s="6">
+      <c r="L10" s="7">
+        <v>1</v>
+      </c>
+      <c r="M10" s="7">
         <v>1</v>
       </c>
       <c r="N10" s="1">
         <v>1</v>
       </c>
-      <c r="O10" s="8">
-        <v>0</v>
-      </c>
-      <c r="P10" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="8">
-        <v>0</v>
-      </c>
-      <c r="R10" s="9"/>
+      <c r="O10" s="7">
+        <v>0</v>
+      </c>
+      <c r="P10" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="7">
+        <v>0</v>
+      </c>
+      <c r="R10" s="8"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>42</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>17</v>
+      <c r="B11" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="C11" s="3">
         <v>30</v>
@@ -1112,32 +1113,32 @@
       <c r="K11" s="2">
         <v>0</v>
       </c>
-      <c r="L11" s="6">
-        <v>1</v>
-      </c>
-      <c r="M11" s="6">
+      <c r="L11" s="7">
+        <v>1</v>
+      </c>
+      <c r="M11" s="7">
         <v>1</v>
       </c>
       <c r="N11" s="1">
         <v>1</v>
       </c>
-      <c r="O11" s="8">
-        <v>0</v>
-      </c>
-      <c r="P11" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="8">
-        <v>0</v>
-      </c>
-      <c r="R11" s="9"/>
+      <c r="O11" s="7">
+        <v>0</v>
+      </c>
+      <c r="P11" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="7">
+        <v>0</v>
+      </c>
+      <c r="R11" s="8"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>76</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>18</v>
+      <c r="B12" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="C12" s="3">
         <v>27</v>
@@ -1166,32 +1167,32 @@
       <c r="K12" s="2">
         <v>0</v>
       </c>
-      <c r="L12" s="6">
-        <v>0</v>
-      </c>
-      <c r="M12" s="6">
+      <c r="L12" s="7">
+        <v>0</v>
+      </c>
+      <c r="M12" s="7">
         <v>0</v>
       </c>
       <c r="N12" s="1">
         <v>0</v>
       </c>
-      <c r="O12" s="8">
-        <v>0</v>
-      </c>
-      <c r="P12" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="8">
-        <v>0</v>
-      </c>
-      <c r="R12" s="10"/>
+      <c r="O12" s="7">
+        <v>0</v>
+      </c>
+      <c r="P12" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="7">
+        <v>0</v>
+      </c>
+      <c r="R12" s="9"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>120</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>19</v>
+      <c r="B13" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="C13" s="3">
         <v>25</v>
@@ -1220,32 +1221,32 @@
       <c r="K13" s="2">
         <v>0</v>
       </c>
-      <c r="L13" s="6">
-        <v>0</v>
-      </c>
-      <c r="M13" s="6">
+      <c r="L13" s="7">
+        <v>0</v>
+      </c>
+      <c r="M13" s="7">
         <v>0</v>
       </c>
       <c r="N13" s="1">
         <v>0</v>
       </c>
-      <c r="O13" s="8">
-        <v>0</v>
-      </c>
-      <c r="P13" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="8">
-        <v>0</v>
-      </c>
-      <c r="R13" s="10"/>
+      <c r="O13" s="7">
+        <v>0</v>
+      </c>
+      <c r="P13" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="7">
+        <v>0</v>
+      </c>
+      <c r="R13" s="9"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>139</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>20</v>
+      <c r="B14" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="C14" s="3">
         <v>29</v>
@@ -1274,32 +1275,32 @@
       <c r="K14" s="2">
         <v>0</v>
       </c>
-      <c r="L14" s="6">
-        <v>0</v>
-      </c>
-      <c r="M14" s="6">
+      <c r="L14" s="7">
+        <v>0</v>
+      </c>
+      <c r="M14" s="7">
         <v>0</v>
       </c>
       <c r="N14" s="1">
         <v>0</v>
       </c>
-      <c r="O14" s="8">
-        <v>0</v>
-      </c>
-      <c r="P14" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="8">
-        <v>0</v>
-      </c>
-      <c r="R14" s="10"/>
+      <c r="O14" s="7">
+        <v>0</v>
+      </c>
+      <c r="P14" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="7">
+        <v>0</v>
+      </c>
+      <c r="R14" s="9"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>148</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>21</v>
+      <c r="B15" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="C15" s="3">
         <v>28</v>
@@ -1328,32 +1329,32 @@
       <c r="K15" s="2">
         <v>0</v>
       </c>
-      <c r="L15" s="6">
-        <v>1</v>
-      </c>
-      <c r="M15" s="6">
+      <c r="L15" s="7">
+        <v>1</v>
+      </c>
+      <c r="M15" s="7">
         <v>1</v>
       </c>
       <c r="N15" s="1">
         <v>0</v>
       </c>
-      <c r="O15" s="8">
-        <v>0</v>
-      </c>
-      <c r="P15" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="8">
-        <v>1</v>
-      </c>
-      <c r="R15" s="9"/>
+      <c r="O15" s="7">
+        <v>0</v>
+      </c>
+      <c r="P15" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="7">
+        <v>1</v>
+      </c>
+      <c r="R15" s="8"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>156</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>22</v>
+      <c r="B16" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="C16" s="3">
         <v>31</v>
@@ -1382,32 +1383,32 @@
       <c r="K16" s="2">
         <v>0</v>
       </c>
-      <c r="L16" s="6">
-        <v>1</v>
-      </c>
-      <c r="M16" s="6">
+      <c r="L16" s="7">
+        <v>1</v>
+      </c>
+      <c r="M16" s="7">
         <v>1</v>
       </c>
       <c r="N16" s="1">
         <v>0</v>
       </c>
-      <c r="O16" s="8">
-        <v>0</v>
-      </c>
-      <c r="P16" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="8">
-        <v>0</v>
-      </c>
-      <c r="R16" s="9"/>
+      <c r="O16" s="7">
+        <v>0</v>
+      </c>
+      <c r="P16" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="7">
+        <v>0</v>
+      </c>
+      <c r="R16" s="8"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>160</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>23</v>
+      <c r="B17" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="C17" s="3">
         <v>29</v>
@@ -1436,32 +1437,32 @@
       <c r="K17" s="4">
         <v>1</v>
       </c>
-      <c r="L17" s="6">
-        <v>0</v>
-      </c>
-      <c r="M17" s="6">
+      <c r="L17" s="7">
+        <v>0</v>
+      </c>
+      <c r="M17" s="7">
         <v>0</v>
       </c>
       <c r="N17" s="1">
         <v>0</v>
       </c>
-      <c r="O17" s="8">
-        <v>0</v>
-      </c>
-      <c r="P17" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="8">
-        <v>0</v>
-      </c>
-      <c r="R17" s="10"/>
+      <c r="O17" s="7">
+        <v>0</v>
+      </c>
+      <c r="P17" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="7">
+        <v>0</v>
+      </c>
+      <c r="R17" s="9"/>
     </row>
     <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>170</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>24</v>
+      <c r="B18" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="C18" s="3">
         <v>30</v>
@@ -1490,25 +1491,25 @@
       <c r="K18" s="2">
         <v>0</v>
       </c>
-      <c r="L18" s="6">
-        <v>1</v>
-      </c>
-      <c r="M18" s="6">
+      <c r="L18" s="7">
+        <v>1</v>
+      </c>
+      <c r="M18" s="7">
         <v>0</v>
       </c>
       <c r="N18" s="1">
         <v>0</v>
       </c>
-      <c r="O18" s="8">
-        <v>0</v>
-      </c>
-      <c r="P18" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="8">
-        <v>1</v>
-      </c>
-      <c r="R18" s="9"/>
+      <c r="O18" s="7">
+        <v>0</v>
+      </c>
+      <c r="P18" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="7">
+        <v>1</v>
+      </c>
+      <c r="R18" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>